<commit_message>
[Fix] Corrections Lot1 et lot2
</commit_message>
<xml_diff>
--- a/lot2/results/Analysed_Datalot2.xlsx
+++ b/lot2/results/Analysed_Datalot2.xlsx
@@ -369,83 +369,83 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Avg_Quantity</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>City</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Timbre</t>
-        </is>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>TRELAZE</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>1593</v>
+      <c r="A2" t="n">
+        <v>77.75</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ECOUFLANT</t>
+        </is>
       </c>
       <c r="C2" t="n">
-        <v>22</v>
+        <v>933</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>SAINT BERTHEVIN</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>921</v>
+      <c r="A3" t="n">
+        <v>66.78571428571429</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>MONTIGNE LE BRILLANT</t>
+        </is>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>935</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>ST BRANDAN</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>919</v>
+      <c r="A4" t="n">
+        <v>92</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>LES GARENNES SUR LOIRE</t>
+        </is>
       </c>
       <c r="C4" t="n">
-        <v>13</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>OLIVET</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1780</v>
+      <c r="A5" t="n">
+        <v>64.1025641025641</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>RENAZE</t>
+        </is>
       </c>
       <c r="C5" t="n">
-        <v>19</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>VALANJOU</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>1457</v>
+      <c r="A6" t="n">
+        <v>90.29166666666667</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>TORCE VIVIERS EN CHARNIE</t>
+        </is>
       </c>
       <c r="C6" t="n">
-        <v>20</v>
+        <v>2167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>